<commit_message>
Proposed Vendor Onboarding Process and Vendor Version of website. See todo in StallPage.jsx for next steps
</commit_message>
<xml_diff>
--- a/TestExcelBooks/Book1.xlsx
+++ b/TestExcelBooks/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaredsmith/Desktop/UNLV/2025_Fall/CS 472- Software Product Design/Assignments/2nd GitAssignment /SeniorDesignProject/TestExcelBooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A707C42F-EEFD-B944-9D61-3D7E7A9F1C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C53F2F5-F679-EA41-8CCE-9472D5C79265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5840" yWindow="5860" windowWidth="28040" windowHeight="17180" xr2:uid="{DD741F2F-2F75-E145-B917-4F90C4CF4640}"/>
   </bookViews>
@@ -38,12 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
-    <t>name</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
     <t>Vendor1</t>
   </si>
   <si>
@@ -96,6 +90,12 @@
   </si>
   <si>
     <t>Vendor9</t>
+  </si>
+  <si>
+    <t>vendor0@email.com</t>
+  </si>
+  <si>
+    <t>Vendor0</t>
   </si>
 </sst>
 </file>
@@ -480,9 +480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB408971-C52E-324D-A90C-5FF789336685}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -491,95 +489,96 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+        <v>19</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{8A360E85-C774-F44D-81BA-61B09FD37F88}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{724CD0E1-BD32-4C4F-A3D1-2E669751898D}"/>
-    <hyperlink ref="B4" r:id="rId3" xr:uid="{094B82A7-57F0-0A43-8564-3B27D198AD93}"/>
-    <hyperlink ref="B5" r:id="rId4" xr:uid="{08ABCDE3-CE3D-6C42-82AD-6D9FC8BF7484}"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{7444207D-2F19-094A-8E34-F28C9A394639}"/>
+    <hyperlink ref="B9" r:id="rId2" xr:uid="{105E1524-4612-0141-824B-71ADFE482CDD}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{236B4A66-44CA-A243-9B6D-98AC2FB3BD25}"/>
+    <hyperlink ref="B7" r:id="rId4" xr:uid="{FEA3B5C3-9D60-1045-8D98-6506E9BC2FEF}"/>
     <hyperlink ref="B6" r:id="rId5" xr:uid="{96BFA454-906F-F54F-B105-0A47D455E0E2}"/>
-    <hyperlink ref="B7" r:id="rId6" xr:uid="{FEA3B5C3-9D60-1045-8D98-6506E9BC2FEF}"/>
-    <hyperlink ref="B8" r:id="rId7" xr:uid="{236B4A66-44CA-A243-9B6D-98AC2FB3BD25}"/>
-    <hyperlink ref="B9" r:id="rId8" xr:uid="{105E1524-4612-0141-824B-71ADFE482CDD}"/>
-    <hyperlink ref="B10" r:id="rId9" xr:uid="{7444207D-2F19-094A-8E34-F28C9A394639}"/>
+    <hyperlink ref="B5" r:id="rId6" xr:uid="{08ABCDE3-CE3D-6C42-82AD-6D9FC8BF7484}"/>
+    <hyperlink ref="B4" r:id="rId7" xr:uid="{094B82A7-57F0-0A43-8564-3B27D198AD93}"/>
+    <hyperlink ref="B3" r:id="rId8" xr:uid="{724CD0E1-BD32-4C4F-A3D1-2E669751898D}"/>
+    <hyperlink ref="B2" r:id="rId9" xr:uid="{8A360E85-C774-F44D-81BA-61B09FD37F88}"/>
+    <hyperlink ref="B1" r:id="rId10" xr:uid="{FB7971B1-A626-B146-B61A-C65B2D923D55}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>